<commit_message>
Cambios al 7 de junio
Se aceptaron cambios de CCC
Se reviso GE 1 y 2 luego de comentarios de Dino
Se reviso que no existieran títulos sueltos en el documento
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
-  <si>
-    <t>1. Analisis (Identificar)</t>
-  </si>
-  <si>
-    <t>1.1 Analisis Corportativo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>1.1.1 Objetivos Corporativos</t>
   </si>
@@ -44,33 +38,18 @@
     <t>1.1.4 Desafios y Limitaciones</t>
   </si>
   <si>
-    <t>1.2 Analisis del Usuario</t>
-  </si>
-  <si>
     <t>1.2.1 Usuarios Finales</t>
   </si>
   <si>
-    <t>1.2.2. Objetivos de Usuarios</t>
-  </si>
-  <si>
     <t>1.2.3 Experiencia y Entorno</t>
   </si>
   <si>
-    <t>1.3 Analisis del Sistema</t>
-  </si>
-  <si>
-    <t>1.3.1. Arquitectura de la Información</t>
-  </si>
-  <si>
     <t>1.3.2 Flujo</t>
   </si>
   <si>
     <t>1.3.3 Benchmarking</t>
   </si>
   <si>
-    <t>1.3.4 Storyboard</t>
-  </si>
-  <si>
     <t>2. Diseño</t>
   </si>
   <si>
@@ -114,13 +93,34 @@
   </si>
   <si>
     <t>Actividad</t>
+  </si>
+  <si>
+    <t>1.3.4 Desarrollar Storyboard</t>
+  </si>
+  <si>
+    <t>1. Análisis (Identificar)</t>
+  </si>
+  <si>
+    <t>1.1 Análisis Corportativo</t>
+  </si>
+  <si>
+    <t>1.2 Análisis del Usuario</t>
+  </si>
+  <si>
+    <t>1.3 Análisis del Sistema</t>
+  </si>
+  <si>
+    <t>1.3.1 Arquitectura de la Información</t>
+  </si>
+  <si>
+    <t>1.2.2 Objetivos de Usuarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +141,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -156,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -181,7 +189,295 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
         <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
       </left>
       <right style="thin">
         <color theme="0"/>
@@ -189,20 +485,37 @@
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7030A0"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7030A0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF7030A0"/>
       </bottom>
       <diagonal/>
@@ -211,17 +524,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,96 +847,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L30"/>
+  <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="5">
+      <c r="B2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="25">
         <v>2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="25">
         <v>3</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="25">
         <v>4</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="25">
         <v>5</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="25">
         <v>6</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="25">
         <v>7</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="25">
         <v>8</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="25">
         <v>9</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="26">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
+      <c r="B5" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -598,14 +947,14 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>2</v>
+      <c r="B6" s="11" t="s">
+        <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -615,14 +964,14 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+      <c r="B7" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -632,14 +981,14 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+      <c r="B8" s="11" t="s">
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -649,14 +998,14 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>5</v>
+      <c r="B9" s="11" t="s">
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -666,15 +1015,15 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>6</v>
+      <c r="B10" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -683,15 +1032,15 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>7</v>
+      <c r="B11" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -700,15 +1049,15 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>8</v>
+      <c r="B12" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -717,15 +1066,15 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>9</v>
+      <c r="B13" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -734,16 +1083,16 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>10</v>
+      <c r="B14" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -751,16 +1100,16 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>11</v>
+      <c r="B15" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -768,16 +1117,16 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>12</v>
+      <c r="B16" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -785,16 +1134,16 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>13</v>
+      <c r="B17" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -802,119 +1151,135 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="B19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>16</v>
+      <c r="B20" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>17</v>
+      <c r="B21" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="B23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>20</v>
+      <c r="B24" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -923,15 +1288,17 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>21</v>
+      <c r="B25" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -940,15 +1307,17 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>22</v>
+      <c r="B26" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -956,97 +1325,101 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J26" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>24</v>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="16"/>
+    </row>
+    <row r="29" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios al 17 de Julio del 2017
Ya todos los cambios hechos para mandar a CIE. Enmienda enviada
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>1.1.1 Objetivos Corporativos</t>
   </si>
@@ -53,15 +53,6 @@
     <t>2. Diseño</t>
   </si>
   <si>
-    <t>2.1 Wireframe</t>
-  </si>
-  <si>
-    <t>2.2 Mockup</t>
-  </si>
-  <si>
-    <t>2.3 Prototyping</t>
-  </si>
-  <si>
     <t>3. Evaluación</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>Actividad</t>
   </si>
   <si>
-    <t>1.3.4 Desarrollar Storyboard</t>
-  </si>
-  <si>
     <t>1. Análisis (Identificar)</t>
   </si>
   <si>
@@ -114,6 +102,21 @@
   </si>
   <si>
     <t>1.2.2 Objetivos de Usuarios</t>
+  </si>
+  <si>
+    <t>1.3.4 Creación de 'Personas'</t>
+  </si>
+  <si>
+    <t>2.1 Storyboard</t>
+  </si>
+  <si>
+    <t>2.2 Wireframe</t>
+  </si>
+  <si>
+    <t>2.3 Mockup</t>
+  </si>
+  <si>
+    <t>2.4 Prototyping</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -520,11 +523,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -556,20 +598,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L30"/>
+  <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,67 +909,67 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="23"/>
+      <c r="B2" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="21">
         <v>1</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="21">
         <v>2</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="21">
         <v>3</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="21">
         <v>4</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="21">
         <v>5</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="21">
         <v>6</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="21">
         <v>7</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="21">
         <v>8</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="21">
         <v>9</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="22">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -934,10 +981,10 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -954,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -971,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -988,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1005,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1019,11 +1066,11 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1040,7 +1087,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1053,11 +1100,11 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1074,7 +1121,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1087,12 +1134,12 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1104,12 +1151,12 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1126,7 +1173,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1143,7 +1190,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1155,12 +1202,12 @@
     </row>
     <row r="18" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1178,127 +1225,127 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="5"/>
+      <c r="B20" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="28"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="F21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="4"/>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="1"/>
-      <c r="L24" s="5"/>
+      <c r="B24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1307,17 +1354,17 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1326,53 +1373,55 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="14"/>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="L28" s="16"/>
+      <c r="B28" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="14"/>
     </row>
     <row r="29" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -1382,44 +1431,61 @@
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="16" t="s">
+      <c r="K29" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="16"/>
+    </row>
+    <row r="30" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L30" s="18" t="s">
-        <v>17</v>
+      <c r="C31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>